<commit_message>
add "Value" column to Excel file
</commit_message>
<xml_diff>
--- a/vavAO_list.xlsx
+++ b/vavAO_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tmp\OneDrive\Learn\F#\excelDataReader01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tmp\OneDrive\Learn\F#\fsBacnetWrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A2BE43-F3C6-40DA-B39C-7C492AA2DDCB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91CEBCD-339E-4F4C-9573-8C807760EAB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8268" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>ao0</t>
+  </si>
+  <si>
+    <t>ValueToWrite</t>
   </si>
 </sst>
 </file>
@@ -78,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -101,11 +104,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -115,6 +129,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,19 +435,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="10.05078125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.9453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,8 +461,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -457,8 +478,11 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -471,8 +495,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -486,7 +513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -498,6 +525,9 @@
       </c>
       <c r="D5">
         <v>3</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>